<commit_message>
data(stations): update thamso_khaithac.xlsx (add/remove stations)
</commit_message>
<xml_diff>
--- a/public/thamso_khaithac.xlsx
+++ b/public/thamso_khaithac.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KT_SL_TTD\DAITRUNGBO\NOIDONGGOI\ktsltd-minimal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KT_SL_TTD\ktsltd-minimal\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="KhaibaoQuangtri" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KhaibaoQuangtri!$A$1:$F$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KhaibaoQuangtri!$A$1:$F$18</definedName>
   </definedNames>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>0</t>
   </si>
@@ -150,40 +150,13 @@
   </si>
   <si>
     <t>matram</t>
-  </si>
-  <si>
-    <t>74445303</t>
-  </si>
-  <si>
-    <t>74445402</t>
-  </si>
-  <si>
-    <t>74445501</t>
-  </si>
-  <si>
-    <t>74445504</t>
-  </si>
-  <si>
-    <t>Thủy văn TĐ Liên Trạch</t>
-  </si>
-  <si>
-    <t>Thủy văn TĐ Lý Hòa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thủy văn TĐ Quảng Phú </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thủy văn TĐ Cao Quảng </t>
-  </si>
-  <si>
-    <t>vrain_mucnuoc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -199,12 +172,6 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF081B3A"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
@@ -271,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -282,13 +249,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -572,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,92 +573,92 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>41</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>555300</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <v>60</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>42</v>
+      <c r="F2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
       </c>
       <c r="E3" s="1">
         <v>60</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>43</v>
+      <c r="F3" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
       </c>
       <c r="E4" s="1">
         <v>60</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>44</v>
+      <c r="F4" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>60</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>34</v>
+      <c r="A6" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -704,12 +669,12 @@
       <c r="E6" s="1">
         <v>60</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B7" t="s">
@@ -724,12 +689,12 @@
       <c r="E7" s="1">
         <v>60</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B8" t="s">
@@ -744,16 +709,16 @@
       <c r="E8" s="1">
         <v>60</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>28</v>
+      <c r="A9" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -764,16 +729,16 @@
       <c r="E9" s="1">
         <v>60</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>26</v>
+      <c r="A10" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -784,19 +749,19 @@
       <c r="E10" s="1">
         <v>60</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>24</v>
+      <c r="A11" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
@@ -804,19 +769,19 @@
       <c r="E11" s="1">
         <v>60</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>22</v>
+      <c r="A12" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
@@ -824,19 +789,19 @@
       <c r="E12" s="1">
         <v>60</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>20</v>
+      <c r="A13" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
@@ -844,19 +809,19 @@
       <c r="E13" s="1">
         <v>60</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>555300</v>
+      <c r="A14" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
@@ -864,16 +829,16 @@
       <c r="E14" s="1">
         <v>60</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
+      <c r="A15" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2">
         <v>2</v>
@@ -884,16 +849,16 @@
       <c r="E15" s="1">
         <v>60</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>15</v>
+      <c r="A16" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2">
         <v>2</v>
@@ -904,16 +869,16 @@
       <c r="E16" s="1">
         <v>60</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>13</v>
+      <c r="A17" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
@@ -924,16 +889,16 @@
       <c r="E17" s="1">
         <v>60</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>11</v>
+      <c r="A18" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C18" s="2">
         <v>2</v>
@@ -944,105 +909,9 @@
       <c r="E18" s="1">
         <v>60</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>60</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="2">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1">
-        <v>60</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="2">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1">
-        <v>60</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="2">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
-        <v>60</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="2"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="2"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="2"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="2"/>
-      <c r="E26" s="1"/>
+      <c r="F18" s="4" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>